<commit_message>
added audio to Votlo (Epi)
</commit_message>
<xml_diff>
--- a/raw/data/Votlo/Votlo.xlsx
+++ b/raw/data/Votlo/Votlo.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Desktop/VV/raw/sandrine2/Volto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/DLCE/lexibank/vanuatuvoices/raw/data/Votlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77F7D276-A912-E741-9F52-89C0DCF9CC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76995E9F-DF25-B449-9D43-2642DE62031D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{3C236B71-7E54-5C4A-A638-17F3CA17EF40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="630">
   <si>
     <t>hand</t>
   </si>
@@ -1917,6 +1917,12 @@
   </si>
   <si>
     <t>Volto</t>
+  </si>
+  <si>
+    <t>wom/hot</t>
+  </si>
+  <si>
+    <t>leik</t>
   </si>
 </sst>
 </file>
@@ -2270,8 +2276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6791D79B-F657-9A4B-8DA3-66651C31C9D3}">
   <dimension ref="A1:C214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="G131" sqref="G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3663,7 +3669,7 @@
         <v>365</v>
       </c>
       <c r="C126" t="s">
-        <v>10</v>
+        <v>629</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -3795,7 +3801,7 @@
         <v>400</v>
       </c>
       <c r="C138" t="s">
-        <v>310</v>
+        <v>628</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>